<commit_message>
Follow change of xlsx.js 2.0.0.
</commit_message>
<xml_diff>
--- a/test/testref/save.xlsx
+++ b/test/testref/save.xlsx
@@ -30,11 +30,6 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="3">
-    <numFmt formatCode="GENERAL" numFmtId="164"/>
-    <numFmt formatCode="GENERAL" numFmtId="165"/>
-    <numFmt formatCode="YYYY/MM/DD" numFmtId="166"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -64,8 +59,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="5" borderId="0" fillId="0" fontId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" borderId="0" fillId="0" fontId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -393,8 +390,8 @@
       <c r="A3">
         <v>1.234</v>
       </c>
-      <c r="B3" s="1" t="n">
-        <v>41202</v>
+      <c r="B3" s="2">
+        <v>41194.375</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add xml-escaping for sheet-name and cell-value.
</commit_message>
<xml_diff>
--- a/test/testref/save.xlsx
+++ b/test/testref/save.xlsx
@@ -8,16 +8,23 @@
   </bookViews>
   <sheets>
     <sheet name="sheet_1" sheetId="1" r:id="rId1"/>
-    <sheet name="sheet_2" sheetId="2" r:id="rId2"/>
+    <sheet name="シート&lt;2&gt;" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>AAAAA</t>
+  </si>
+  <si>
+    <t>&lt;&gt;"'&amp;</t>
+  </si>
+  <si>
+    <t>a
+b</t>
   </si>
   <si>
     <t>ABC</t>
@@ -375,7 +382,7 @@
         <v>10</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -383,7 +390,7 @@
         <v>-10</v>
       </c>
       <c r="B2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -401,7 +408,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -415,6 +422,14 @@
         <v>0</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Follow xlsx.js vervion 2.2.0.
</commit_message>
<xml_diff>
--- a/test/testref/save.xlsx
+++ b/test/testref/save.xlsx
@@ -377,7 +377,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>10</v>
       </c>
@@ -385,7 +385,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-10</v>
       </c>
@@ -393,7 +393,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1.234</v>
       </c>
@@ -414,7 +414,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>9999</v>
       </c>
@@ -422,7 +422,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>

</xml_diff>

<commit_message>
Update for xlsx.js ver 2.3.0
</commit_message>
<xml_diff>
--- a/test/testref/save.xlsx
+++ b/test/testref/save.xlsx
@@ -68,8 +68,8 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="5" borderId="0" fillId="0" fontId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="14" borderId="0" fillId="0" fontId="0" xfId="0" applyNumberFormat="1"/>
+    <xf xfId="0" fillId="0" borderId="0" fontId="0" numFmtId="0"/>
+    <xf xfId="0" fillId="0" borderId="0" fontId="0" numFmtId="14" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -378,27 +378,27 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>10</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>-10</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1.234</v>
       </c>
       <c r="B3" s="2">
-        <v>41192</v>
+        <v>41194.375</v>
       </c>
     </row>
   </sheetData>
@@ -415,18 +415,18 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" x14ac:dyDescent="0.25">
-      <c r="A1">
+      <c r="A1" s="1">
         <v>9999</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>